<commit_message>
Update mail, registration link and list of committee members of BBS SR
</commit_message>
<xml_diff>
--- a/data/roster_romandie.xlsx
+++ b/data/roster_romandie.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edupuisl\OneDrive - Philip Morris International\BBS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pmicloud-my.sharepoint.com/personal/edupuisl_pmintl_net/Documents/BBS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{EAF48032-AC1C-4986-A3D7-89776110E89C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F7416586-AFD1-4778-9E22-445D825675E2}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{D942393C-CAD1-4619-A9EF-42247D71E15A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{024BE14E-CDC4-4584-84B2-A88E90E3BA09}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="4850" xr2:uid="{85CC347E-63AB-4647-8E5F-A9DE4D99A9F5}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$E$16</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$E$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>First</t>
   </si>
@@ -99,18 +99,6 @@
     <t>Korneliou</t>
   </si>
   <si>
-    <t>Dea</t>
-  </si>
-  <si>
-    <t>Putri</t>
-  </si>
-  <si>
-    <t>Marco</t>
-  </si>
-  <si>
-    <t>Eigenmann</t>
-  </si>
-  <si>
     <t>Alessandro</t>
   </si>
   <si>
@@ -166,6 +154,15 @@
   </si>
   <si>
     <t>Statistician/Consultant</t>
+  </si>
+  <si>
+    <t>Laura-Florina</t>
+  </si>
+  <si>
+    <t>Krattinger</t>
+  </si>
+  <si>
+    <t>Nestlé</t>
   </si>
 </sst>
 </file>
@@ -253,10 +250,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25C48855-235A-4A93-AB37-5D4A2F58AB3D}" name="roster_romandie" displayName="roster_romandie" ref="A1:E16" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E16" xr:uid="{A940EF7D-6009-4ECD-B6E3-DAB438BAF116}"/>
-  <sortState ref="A2:E16">
-    <sortCondition ref="B2:B16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25C48855-235A-4A93-AB37-5D4A2F58AB3D}" name="roster_romandie" displayName="roster_romandie" ref="A1:E15" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:E15" xr:uid="{A940EF7D-6009-4ECD-B6E3-DAB438BAF116}"/>
+  <sortState ref="A2:E14">
+    <sortCondition ref="B2:B14"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9285C058-128C-4C6F-A7FB-03B5F32CF77F}" uniqueName="1" name="First" queryTableFieldId="1" dataDxfId="3"/>
@@ -566,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADCEB3A-F945-4725-BC6C-5E6712111CB7}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="N12" sqref="N11:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,7 +578,7 @@
     <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -598,12 +595,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -613,22 +610,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -645,7 +642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -662,7 +659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -679,12 +676,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
@@ -696,12 +693,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -713,15 +710,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -730,47 +727,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="1"/>
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>8</v>
@@ -778,77 +776,60 @@
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="D15" s="1"/>
       <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -869,23 +850,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="98da23c0-7a35-4b8a-8aee-b4cdeb3e7e52" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B723A697A77354F857C3D6DA304BA94" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d42aa8a23f07d1c51f7c277388e902d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="98da23c0-7a35-4b8a-8aee-b4cdeb3e7e52" xmlns:ns4="b2f47ca5-43fa-4a5a-ac50-58eca229e588" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e0dfb2e5d95cd1c4d8747abc33a7f2b6" ns3:_="" ns4:_="">
     <xsd:import namespace="98da23c0-7a35-4b8a-8aee-b4cdeb3e7e52"/>
@@ -1126,6 +1090,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="98da23c0-7a35-4b8a-8aee-b4cdeb3e7e52" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0880BD0-01CE-454D-B12C-CFAAC107F3D3}">
   <ds:schemaRefs>
@@ -1135,31 +1116,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA4F269-3C3E-494B-84AF-C3327A3A6414}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="98da23c0-7a35-4b8a-8aee-b4cdeb3e7e52"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b2f47ca5-43fa-4a5a-ac50-58eca229e588"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F84823E8-71AB-4A1A-9EE6-6AC03FC719C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE8CA331-6094-4024-B8F6-5C6056C670A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1176,4 +1132,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F84823E8-71AB-4A1A-9EE6-6AC03FC719C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA4F269-3C3E-494B-84AF-C3327A3A6414}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b2f47ca5-43fa-4a5a-ac50-58eca229e588"/>
+    <ds:schemaRef ds:uri="98da23c0-7a35-4b8a-8aee-b4cdeb3e7e52"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Update mail, registration link and list of committee members of BBS SR"
</commit_message>
<xml_diff>
--- a/data/roster_romandie.xlsx
+++ b/data/roster_romandie.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pmicloud-my.sharepoint.com/personal/edupuisl_pmintl_net/Documents/BBS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edupuisl\OneDrive - Philip Morris International\BBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{D942393C-CAD1-4619-A9EF-42247D71E15A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{024BE14E-CDC4-4584-84B2-A88E90E3BA09}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{EAF48032-AC1C-4986-A3D7-89776110E89C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F7416586-AFD1-4778-9E22-445D825675E2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="4850" xr2:uid="{85CC347E-63AB-4647-8E5F-A9DE4D99A9F5}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$E$15</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$E$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>First</t>
   </si>
@@ -99,6 +99,18 @@
     <t>Korneliou</t>
   </si>
   <si>
+    <t>Dea</t>
+  </si>
+  <si>
+    <t>Putri</t>
+  </si>
+  <si>
+    <t>Marco</t>
+  </si>
+  <si>
+    <t>Eigenmann</t>
+  </si>
+  <si>
     <t>Alessandro</t>
   </si>
   <si>
@@ -154,15 +166,6 @@
   </si>
   <si>
     <t>Statistician/Consultant</t>
-  </si>
-  <si>
-    <t>Laura-Florina</t>
-  </si>
-  <si>
-    <t>Krattinger</t>
-  </si>
-  <si>
-    <t>Nestlé</t>
   </si>
 </sst>
 </file>
@@ -250,10 +253,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25C48855-235A-4A93-AB37-5D4A2F58AB3D}" name="roster_romandie" displayName="roster_romandie" ref="A1:E15" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E15" xr:uid="{A940EF7D-6009-4ECD-B6E3-DAB438BAF116}"/>
-  <sortState ref="A2:E14">
-    <sortCondition ref="B2:B14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25C48855-235A-4A93-AB37-5D4A2F58AB3D}" name="roster_romandie" displayName="roster_romandie" ref="A1:E16" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:E16" xr:uid="{A940EF7D-6009-4ECD-B6E3-DAB438BAF116}"/>
+  <sortState ref="A2:E16">
+    <sortCondition ref="B2:B16"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9285C058-128C-4C6F-A7FB-03B5F32CF77F}" uniqueName="1" name="First" queryTableFieldId="1" dataDxfId="3"/>
@@ -563,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADCEB3A-F945-4725-BC6C-5E6712111CB7}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N11:N12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -578,7 +581,7 @@
     <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -595,12 +598,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -610,22 +613,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -642,7 +645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -659,7 +662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -676,12 +679,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
@@ -693,12 +696,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -710,15 +713,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -727,48 +730,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>8</v>
@@ -776,60 +778,77 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="E13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15">
+      <c r="E16">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -850,6 +869,23 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="98da23c0-7a35-4b8a-8aee-b4cdeb3e7e52" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B723A697A77354F857C3D6DA304BA94" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d42aa8a23f07d1c51f7c277388e902d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="98da23c0-7a35-4b8a-8aee-b4cdeb3e7e52" xmlns:ns4="b2f47ca5-43fa-4a5a-ac50-58eca229e588" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e0dfb2e5d95cd1c4d8747abc33a7f2b6" ns3:_="" ns4:_="">
     <xsd:import namespace="98da23c0-7a35-4b8a-8aee-b4cdeb3e7e52"/>
@@ -1090,23 +1126,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="98da23c0-7a35-4b8a-8aee-b4cdeb3e7e52" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0880BD0-01CE-454D-B12C-CFAAC107F3D3}">
   <ds:schemaRefs>
@@ -1116,6 +1135,31 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA4F269-3C3E-494B-84AF-C3327A3A6414}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="98da23c0-7a35-4b8a-8aee-b4cdeb3e7e52"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b2f47ca5-43fa-4a5a-ac50-58eca229e588"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F84823E8-71AB-4A1A-9EE6-6AC03FC719C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE8CA331-6094-4024-B8F6-5C6056C670A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1132,29 +1176,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F84823E8-71AB-4A1A-9EE6-6AC03FC719C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA4F269-3C3E-494B-84AF-C3327A3A6414}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b2f47ca5-43fa-4a5a-ac50-58eca229e588"/>
-    <ds:schemaRef ds:uri="98da23c0-7a35-4b8a-8aee-b4cdeb3e7e52"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>